<commit_message>
Add CSV metadata to infrastructure-costs files
- Add column width and alignment metadata rows to all sections
- Update solution template and AWS IDP infrastructure-costs CSV files
- Regenerate Excel files with updated converter supporting metadata
- Ensure consistent formatting with metadata-driven column widths
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/presales/infrastructure-costs.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/presales/infrastructure-costs.xlsx
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -319,9 +319,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -335,9 +332,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -347,32 +341,47 @@
     <xf numFmtId="9" fontId="11" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -384,22 +393,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -408,10 +423,10 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="17" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -427,12 +442,6 @@
     </xf>
     <xf numFmtId="165" fontId="19" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,14 +796,14 @@
     </row>
     <row r="2" ht="15" customHeight="1"/>
     <row r="3" ht="40" customHeight="1">
-      <c r="B3" s="17" t="inlineStr">
+      <c r="B3" s="16" t="inlineStr">
         <is>
           <t>[DOCUMENT TITLE]</t>
         </is>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1">
-      <c r="B4" s="16" t="inlineStr">
+      <c r="B4" s="15" t="inlineStr">
         <is>
           <t>Infrastructure Costs</t>
         </is>
@@ -905,263 +914,263 @@
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>Sizing Guidelines</t>
         </is>
       </c>
     </row>
     <row r="2" ht="32" customHeight="1">
-      <c r="A2" s="33" t="inlineStr">
+      <c r="A2" s="36" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B2" s="33" t="inlineStr">
+      <c r="B2" s="36" t="inlineStr">
         <is>
           <t>Component</t>
         </is>
       </c>
-      <c r="C2" s="33" t="inlineStr">
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
       </c>
-      <c r="D2" s="33" t="inlineStr">
+      <c r="D2" s="36" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E2" s="33" t="inlineStr">
+      <c r="E2" s="36" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
       </c>
-      <c r="F2" s="33" t="inlineStr">
+      <c r="F2" s="36" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="3" ht="26" customHeight="1">
-      <c r="A3" s="34" t="inlineStr">
+      <c r="A3" s="37" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B3" s="35" t="inlineStr">
+      <c r="B3" s="38" t="inlineStr">
         <is>
           <t>Compute Instances</t>
         </is>
       </c>
-      <c r="C3" s="35" t="inlineStr">
+      <c r="C3" s="39" t="inlineStr">
         <is>
           <t>2-4 instances</t>
         </is>
       </c>
-      <c r="D3" s="35" t="inlineStr">
+      <c r="D3" s="39" t="inlineStr">
         <is>
           <t>5-10 instances</t>
         </is>
       </c>
-      <c r="E3" s="35" t="inlineStr">
+      <c r="E3" s="39" t="inlineStr">
         <is>
           <t>15+ instances</t>
         </is>
       </c>
-      <c r="F3" s="35" t="inlineStr">
+      <c r="F3" s="38" t="inlineStr">
         <is>
           <t>Production workload capacity</t>
         </is>
       </c>
     </row>
     <row r="4" ht="26" customHeight="1">
-      <c r="A4" s="36" t="inlineStr">
+      <c r="A4" s="40" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B4" s="37" t="inlineStr">
+      <c r="B4" s="41" t="inlineStr">
         <is>
           <t>Storage Volume</t>
         </is>
       </c>
-      <c r="C4" s="37" t="inlineStr">
+      <c r="C4" s="42" t="inlineStr">
         <is>
           <t>100 GB</t>
         </is>
       </c>
-      <c r="D4" s="37" t="inlineStr">
+      <c r="D4" s="42" t="inlineStr">
         <is>
           <t>500 GB - 1 TB</t>
         </is>
       </c>
-      <c r="E4" s="37" t="inlineStr">
+      <c r="E4" s="42" t="inlineStr">
         <is>
           <t>2+ TB</t>
         </is>
       </c>
-      <c r="F4" s="37" t="inlineStr">
+      <c r="F4" s="41" t="inlineStr">
         <is>
           <t>Based on data requirements</t>
         </is>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
-      <c r="A5" s="34" t="inlineStr">
+      <c r="A5" s="37" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B5" s="35" t="inlineStr">
+      <c r="B5" s="38" t="inlineStr">
         <is>
           <t>Database Size</t>
         </is>
       </c>
-      <c r="C5" s="35" t="inlineStr">
+      <c r="C5" s="39" t="inlineStr">
         <is>
           <t>Small/Standard tier</t>
         </is>
       </c>
-      <c r="D5" s="35" t="inlineStr">
+      <c r="D5" s="39" t="inlineStr">
         <is>
           <t>Medium tier</t>
         </is>
       </c>
-      <c r="E5" s="35" t="inlineStr">
+      <c r="E5" s="39" t="inlineStr">
         <is>
           <t>Large/Enterprise tier</t>
         </is>
       </c>
-      <c r="F5" s="35" t="inlineStr">
+      <c r="F5" s="38" t="inlineStr">
         <is>
           <t>Based on transaction volume</t>
         </is>
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
-      <c r="A6" s="36" t="inlineStr">
+      <c r="A6" s="40" t="inlineStr">
         <is>
           <t>Software Licenses</t>
         </is>
       </c>
-      <c r="B6" s="37" t="inlineStr">
+      <c r="B6" s="41" t="inlineStr">
         <is>
           <t>User Licenses</t>
         </is>
       </c>
-      <c r="C6" s="37" t="inlineStr">
+      <c r="C6" s="42" t="inlineStr">
         <is>
           <t>10-50 users</t>
         </is>
       </c>
-      <c r="D6" s="37" t="inlineStr">
+      <c r="D6" s="42" t="inlineStr">
         <is>
           <t>50-250 users</t>
         </is>
       </c>
-      <c r="E6" s="37" t="inlineStr">
+      <c r="E6" s="42" t="inlineStr">
         <is>
           <t>500+ users</t>
         </is>
       </c>
-      <c r="F6" s="37" t="inlineStr">
+      <c r="F6" s="41" t="inlineStr">
         <is>
           <t>Concurrent or named users</t>
         </is>
       </c>
     </row>
     <row r="7" ht="26" customHeight="1">
-      <c r="A7" s="34" t="inlineStr">
+      <c r="A7" s="37" t="inlineStr">
         <is>
           <t>Software Licenses</t>
         </is>
       </c>
-      <c r="B7" s="35" t="inlineStr">
+      <c r="B7" s="38" t="inlineStr">
         <is>
           <t>Monitoring Tools</t>
         </is>
       </c>
-      <c r="C7" s="35" t="inlineStr">
+      <c r="C7" s="39" t="inlineStr">
         <is>
           <t>Basic monitoring</t>
         </is>
       </c>
-      <c r="D7" s="35" t="inlineStr">
+      <c r="D7" s="39" t="inlineStr">
         <is>
           <t>Advanced APM</t>
         </is>
       </c>
-      <c r="E7" s="35" t="inlineStr">
+      <c r="E7" s="39" t="inlineStr">
         <is>
           <t>Enterprise observability</t>
         </is>
       </c>
-      <c r="F7" s="35" t="inlineStr">
+      <c r="F7" s="38" t="inlineStr">
         <is>
           <t>Application performance monitoring</t>
         </is>
       </c>
     </row>
     <row r="8" ht="26" customHeight="1">
-      <c r="A8" s="36" t="inlineStr">
+      <c r="A8" s="40" t="inlineStr">
         <is>
           <t>Support &amp; Maintenance</t>
         </is>
       </c>
-      <c r="B8" s="37" t="inlineStr">
+      <c r="B8" s="41" t="inlineStr">
         <is>
           <t>Support Level</t>
         </is>
       </c>
-      <c r="C8" s="37" t="inlineStr">
+      <c r="C8" s="42" t="inlineStr">
         <is>
           <t>Business hours</t>
         </is>
       </c>
-      <c r="D8" s="37" t="inlineStr">
+      <c r="D8" s="42" t="inlineStr">
         <is>
           <t>24x5 support</t>
         </is>
       </c>
-      <c r="E8" s="37" t="inlineStr">
+      <c r="E8" s="42" t="inlineStr">
         <is>
           <t>24x7 premium</t>
         </is>
       </c>
-      <c r="F8" s="37" t="inlineStr">
+      <c r="F8" s="41" t="inlineStr">
         <is>
           <t>SLA requirements</t>
         </is>
       </c>
     </row>
     <row r="9" ht="26" customHeight="1">
-      <c r="A9" s="34" t="inlineStr">
+      <c r="A9" s="37" t="inlineStr">
         <is>
           <t>Hardware/Equipment</t>
         </is>
       </c>
-      <c r="B9" s="35" t="inlineStr">
+      <c r="B9" s="38" t="inlineStr">
         <is>
           <t>Network Devices</t>
         </is>
       </c>
-      <c r="C9" s="35" t="inlineStr">
+      <c r="C9" s="39" t="inlineStr">
         <is>
           <t>0-2 devices</t>
         </is>
       </c>
-      <c r="D9" s="35" t="inlineStr">
+      <c r="D9" s="39" t="inlineStr">
         <is>
           <t>3-5 devices</t>
         </is>
       </c>
-      <c r="E9" s="35" t="inlineStr">
+      <c r="E9" s="39" t="inlineStr">
         <is>
           <t>10+ devices</t>
         </is>
       </c>
-      <c r="F9" s="35" t="inlineStr">
+      <c r="F9" s="38" t="inlineStr">
         <is>
           <t>Based on site count</t>
         </is>
@@ -1205,489 +1214,489 @@
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>Infrastructure Costs</t>
         </is>
       </c>
     </row>
     <row r="2" ht="32" customHeight="1">
-      <c r="A2" s="33" t="inlineStr">
+      <c r="A2" s="36" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B2" s="33" t="inlineStr">
+      <c r="B2" s="36" t="inlineStr">
         <is>
           <t>Component</t>
         </is>
       </c>
-      <c r="C2" s="33" t="inlineStr">
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="D2" s="33" t="inlineStr">
+      <c r="D2" s="36" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="E2" s="33" t="inlineStr">
+      <c r="E2" s="36" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="F2" s="33" t="inlineStr">
+      <c r="F2" s="36" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="G2" s="33" t="inlineStr">
+      <c r="G2" s="36" t="inlineStr">
         <is>
           <t>Annual Cost</t>
         </is>
       </c>
-      <c r="H2" s="33" t="inlineStr">
+      <c r="H2" s="36" t="inlineStr">
         <is>
           <t>Year 2</t>
         </is>
       </c>
-      <c r="I2" s="33" t="inlineStr">
+      <c r="I2" s="36" t="inlineStr">
         <is>
           <t>Year 3</t>
         </is>
       </c>
-      <c r="J2" s="33" t="inlineStr">
+      <c r="J2" s="36" t="inlineStr">
         <is>
           <t>3-Year Total</t>
         </is>
       </c>
-      <c r="K2" s="33" t="inlineStr">
+      <c r="K2" s="36" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="20" customHeight="1">
-      <c r="A3" s="38" t="inlineStr">
+    <row r="3" ht="26" customHeight="1">
+      <c r="A3" s="43" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B3" s="39" t="inlineStr">
+      <c r="B3" s="44" t="inlineStr">
         <is>
           <t>Compute Instance</t>
         </is>
       </c>
-      <c r="C3" s="39" t="inlineStr">
+      <c r="C3" s="44" t="inlineStr">
         <is>
           <t>Cloud VM or equivalent</t>
         </is>
       </c>
-      <c r="D3" s="40" t="n">
+      <c r="D3" s="45" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="39" t="inlineStr">
+      <c r="E3" s="44" t="inlineStr">
         <is>
           <t>Instance/Month</t>
         </is>
       </c>
-      <c r="F3" s="41" t="n">
+      <c r="F3" s="46" t="n">
         <v>150</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="46">
         <f>D3*F3*12</f>
         <v/>
       </c>
-      <c r="H3" s="41">
+      <c r="H3" s="46">
         <f>G3</f>
         <v/>
       </c>
-      <c r="I3" s="41">
+      <c r="I3" s="46">
         <f>G3</f>
         <v/>
       </c>
-      <c r="J3" s="41">
+      <c r="J3" s="46">
         <f>G3+H3+I3</f>
         <v/>
       </c>
-      <c r="K3" s="39" t="inlineStr">
+      <c r="K3" s="44" t="inlineStr">
         <is>
           <t>Production workloads</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="42" t="inlineStr">
+    <row r="4" ht="26" customHeight="1">
+      <c r="A4" s="47" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B4" s="43" t="inlineStr">
+      <c r="B4" s="48" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C4" s="43" t="inlineStr">
+      <c r="C4" s="48" t="inlineStr">
         <is>
           <t>Managed database service</t>
         </is>
       </c>
-      <c r="D4" s="44" t="n">
+      <c r="D4" s="49" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="43" t="inlineStr">
+      <c r="E4" s="48" t="inlineStr">
         <is>
           <t>Instance/Month</t>
         </is>
       </c>
-      <c r="F4" s="45" t="n">
+      <c r="F4" s="50" t="n">
         <v>200</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="50">
         <f>D4*F4*12</f>
         <v/>
       </c>
-      <c r="H4" s="45">
+      <c r="H4" s="50">
         <f>G4</f>
         <v/>
       </c>
-      <c r="I4" s="45">
+      <c r="I4" s="50">
         <f>G4</f>
         <v/>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="50">
         <f>G4+H4+I4</f>
         <v/>
       </c>
-      <c r="K4" s="43" t="inlineStr">
+      <c r="K4" s="48" t="inlineStr">
         <is>
           <t>Relational database</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="20" customHeight="1">
-      <c r="A5" s="38" t="inlineStr">
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" s="43" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B5" s="39" t="inlineStr">
+      <c r="B5" s="44" t="inlineStr">
         <is>
           <t>Storage</t>
         </is>
       </c>
-      <c r="C5" s="39" t="inlineStr">
+      <c r="C5" s="44" t="inlineStr">
         <is>
           <t>Object storage</t>
         </is>
       </c>
-      <c r="D5" s="40" t="n">
+      <c r="D5" s="45" t="n">
         <v>100</v>
       </c>
-      <c r="E5" s="39" t="inlineStr">
+      <c r="E5" s="44" t="inlineStr">
         <is>
           <t>GB/Month</t>
         </is>
       </c>
-      <c r="F5" s="41" t="n">
+      <c r="F5" s="46" t="n">
         <v>0.023</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="46">
         <f>D5*F5*12</f>
         <v/>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="46">
         <f>G5</f>
         <v/>
       </c>
-      <c r="I5" s="41">
+      <c r="I5" s="46">
         <f>G5</f>
         <v/>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="46">
         <f>G5+H5+I5</f>
         <v/>
       </c>
-      <c r="K5" s="39" t="inlineStr">
+      <c r="K5" s="44" t="inlineStr">
         <is>
           <t>Data storage</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="42" t="inlineStr">
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" s="47" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B6" s="43" t="inlineStr">
+      <c r="B6" s="48" t="inlineStr">
         <is>
           <t>Data Transfer</t>
         </is>
       </c>
-      <c r="C6" s="43" t="inlineStr">
+      <c r="C6" s="48" t="inlineStr">
         <is>
           <t>Outbound transfer</t>
         </is>
       </c>
-      <c r="D6" s="44" t="n">
+      <c r="D6" s="49" t="n">
         <v>50</v>
       </c>
-      <c r="E6" s="43" t="inlineStr">
+      <c r="E6" s="48" t="inlineStr">
         <is>
           <t>GB/Month</t>
         </is>
       </c>
-      <c r="F6" s="45" t="n">
+      <c r="F6" s="50" t="n">
         <v>0.09</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="50">
         <f>D6*F6*12</f>
         <v/>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="50">
         <f>G6</f>
         <v/>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="50">
         <f>G6</f>
         <v/>
       </c>
-      <c r="J6" s="45">
+      <c r="J6" s="50">
         <f>G6+H6+I6</f>
         <v/>
       </c>
-      <c r="K6" s="43" t="inlineStr">
+      <c r="K6" s="48" t="inlineStr">
         <is>
           <t>Egress charges</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="38" t="inlineStr">
+    <row r="7" ht="26" customHeight="1">
+      <c r="A7" s="43" t="inlineStr">
         <is>
           <t>Software Licenses</t>
         </is>
       </c>
-      <c r="B7" s="39" t="inlineStr">
+      <c r="B7" s="44" t="inlineStr">
         <is>
           <t>Monitoring</t>
         </is>
       </c>
-      <c r="C7" s="39" t="inlineStr">
+      <c r="C7" s="44" t="inlineStr">
         <is>
           <t>Application monitoring</t>
         </is>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="39" t="inlineStr">
+      <c r="E7" s="44" t="inlineStr">
         <is>
           <t>Service/Month</t>
         </is>
       </c>
-      <c r="F7" s="41" t="n">
+      <c r="F7" s="46" t="n">
         <v>50</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="46">
         <f>D7*F7*12</f>
         <v/>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="46">
         <f>G7</f>
         <v/>
       </c>
-      <c r="I7" s="41">
+      <c r="I7" s="46">
         <f>G7</f>
         <v/>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="46">
         <f>G7+H7+I7</f>
         <v/>
       </c>
-      <c r="K7" s="39" t="inlineStr">
+      <c r="K7" s="44" t="inlineStr">
         <is>
           <t>Metrics and logging</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="20" customHeight="1">
-      <c r="A8" s="42" t="inlineStr">
+    <row r="8" ht="26" customHeight="1">
+      <c r="A8" s="47" t="inlineStr">
         <is>
           <t>Software Licenses</t>
         </is>
       </c>
-      <c r="B8" s="43" t="inlineStr">
+      <c r="B8" s="48" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="C8" s="43" t="inlineStr">
+      <c r="C8" s="48" t="inlineStr">
         <is>
           <t>Web application firewall</t>
         </is>
       </c>
-      <c r="D8" s="44" t="n">
+      <c r="D8" s="49" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="43" t="inlineStr">
+      <c r="E8" s="48" t="inlineStr">
         <is>
           <t>Service/Month</t>
         </is>
       </c>
-      <c r="F8" s="45" t="n">
+      <c r="F8" s="50" t="n">
         <v>25</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="50">
         <f>D8*F8*12</f>
         <v/>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="50">
         <f>G8</f>
         <v/>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="50">
         <f>G8</f>
         <v/>
       </c>
-      <c r="J8" s="45">
+      <c r="J8" s="50">
         <f>G8+H8+I8</f>
         <v/>
       </c>
-      <c r="K8" s="43" t="inlineStr">
+      <c r="K8" s="48" t="inlineStr">
         <is>
           <t>Security controls</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="20" customHeight="1">
-      <c r="A9" s="38" t="inlineStr">
+    <row r="9" ht="26" customHeight="1">
+      <c r="A9" s="43" t="inlineStr">
         <is>
           <t>Support &amp; Maintenance</t>
         </is>
       </c>
-      <c r="B9" s="39" t="inlineStr">
+      <c r="B9" s="44" t="inlineStr">
         <is>
           <t>Cloud Support</t>
         </is>
       </c>
-      <c r="C9" s="39" t="inlineStr">
+      <c r="C9" s="44" t="inlineStr">
         <is>
           <t>Provider support plan</t>
         </is>
       </c>
-      <c r="D9" s="40" t="n">
+      <c r="D9" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="39" t="inlineStr">
+      <c r="E9" s="44" t="inlineStr">
         <is>
           <t>Plan/Month</t>
         </is>
       </c>
-      <c r="F9" s="41" t="n">
+      <c r="F9" s="46" t="n">
         <v>100</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="46">
         <f>D9*F9*12</f>
         <v/>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="46">
         <f>G9</f>
         <v/>
       </c>
-      <c r="I9" s="41">
+      <c r="I9" s="46">
         <f>G9</f>
         <v/>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="46">
         <f>G9+H9+I9</f>
         <v/>
       </c>
-      <c r="K9" s="39" t="inlineStr">
+      <c r="K9" s="44" t="inlineStr">
         <is>
           <t>Technical support</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="20" customHeight="1">
-      <c r="A10" s="42" t="inlineStr">
+    <row r="10" ht="26" customHeight="1">
+      <c r="A10" s="47" t="inlineStr">
         <is>
           <t>Hardware/Equipment</t>
         </is>
       </c>
-      <c r="B10" s="43" t="inlineStr">
+      <c r="B10" s="48" t="inlineStr">
         <is>
           <t>Network Switch</t>
         </is>
       </c>
-      <c r="C10" s="43" t="inlineStr">
+      <c r="C10" s="48" t="inlineStr">
         <is>
           <t>Network equipment</t>
         </is>
       </c>
-      <c r="D10" s="44" t="n">
+      <c r="D10" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="43" t="inlineStr">
+      <c r="E10" s="48" t="inlineStr">
         <is>
           <t>Device</t>
         </is>
       </c>
-      <c r="F10" s="45" t="n">
+      <c r="F10" s="50" t="n">
         <v>2500</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="50">
         <f>D10*F10</f>
         <v/>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="50">
         <f>G10</f>
         <v/>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="50">
         <f>G10</f>
         <v/>
       </c>
-      <c r="J10" s="45">
+      <c r="J10" s="50">
         <f>G10+H10+I10</f>
         <v/>
       </c>
-      <c r="K10" s="43" t="inlineStr">
+      <c r="K10" s="48" t="inlineStr">
         <is>
           <t>Optional on-premises</t>
         </is>
       </c>
     </row>
     <row r="11" ht="26" customHeight="1">
-      <c r="A11" s="46" t="inlineStr">
+      <c r="A11" s="51" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B11" s="47" t="n"/>
-      <c r="C11" s="47" t="n"/>
-      <c r="D11" s="47" t="n"/>
-      <c r="E11" s="47" t="n"/>
-      <c r="F11" s="47" t="n"/>
-      <c r="G11" s="48">
+      <c r="B11" s="52" t="n"/>
+      <c r="C11" s="52" t="n"/>
+      <c r="D11" s="52" t="n"/>
+      <c r="E11" s="52" t="n"/>
+      <c r="F11" s="52" t="n"/>
+      <c r="G11" s="53">
         <f>SUM(G3:G10)</f>
         <v/>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="53">
         <f>SUM(H3:H10)</f>
         <v/>
       </c>
-      <c r="I11" s="48">
+      <c r="I11" s="53">
         <f>SUM(I3:I10)</f>
         <v/>
       </c>
-      <c r="J11" s="48">
+      <c r="J11" s="53">
         <f>SUM(J3:J10)</f>
         <v/>
       </c>
-      <c r="K11" s="47" t="n"/>
+      <c r="K11" s="52" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:K11"/>
@@ -1720,109 +1729,109 @@
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>Credits</t>
         </is>
       </c>
     </row>
     <row r="2" ht="32" customHeight="1">
-      <c r="A2" s="33" t="inlineStr">
+      <c r="A2" s="36" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B2" s="33" t="inlineStr">
+      <c r="B2" s="36" t="inlineStr">
         <is>
           <t>Credit Type</t>
         </is>
       </c>
-      <c r="C2" s="33" t="inlineStr">
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>Credit Amount</t>
         </is>
       </c>
-      <c r="D2" s="33" t="inlineStr">
+      <c r="D2" s="36" t="inlineStr">
         <is>
           <t>Credit Comments</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="20" customHeight="1">
-      <c r="A3" s="38" t="inlineStr">
+    <row r="3" ht="26" customHeight="1">
+      <c r="A3" s="43" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B3" s="49" t="inlineStr">
+      <c r="B3" s="44" t="inlineStr">
         <is>
           <t>Provider Credit</t>
         </is>
       </c>
-      <c r="C3" s="41" t="n">
+      <c r="C3" s="46" t="n">
         <v>-1800</v>
       </c>
-      <c r="D3" s="49" t="inlineStr">
+      <c r="D3" s="44" t="inlineStr">
         <is>
           <t>30% credit on eligible compute and database services</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="42" t="inlineStr">
+    <row r="4" ht="26" customHeight="1">
+      <c r="A4" s="47" t="inlineStr">
         <is>
           <t>Software Licenses</t>
         </is>
       </c>
-      <c r="B4" s="50" t="inlineStr">
+      <c r="B4" s="48" t="inlineStr">
         <is>
           <t>Partner Credit</t>
         </is>
       </c>
-      <c r="C4" s="45" t="n">
+      <c r="C4" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="50" t="inlineStr">
+      <c r="D4" s="48" t="inlineStr">
         <is>
           <t>No software credits available</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="20" customHeight="1">
-      <c r="A5" s="38" t="inlineStr">
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" s="43" t="inlineStr">
         <is>
           <t>Support &amp; Maintenance</t>
         </is>
       </c>
-      <c r="B5" s="49" t="inlineStr">
+      <c r="B5" s="44" t="inlineStr">
         <is>
           <t>Program Credit</t>
         </is>
       </c>
-      <c r="C5" s="41" t="n">
+      <c r="C5" s="46" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="49" t="inlineStr">
+      <c r="D5" s="44" t="inlineStr">
         <is>
           <t>No support credits available</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="42" t="inlineStr">
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" s="47" t="inlineStr">
         <is>
           <t>Hardware/Equipment</t>
         </is>
       </c>
-      <c r="B6" s="50" t="inlineStr">
+      <c r="B6" s="48" t="inlineStr">
         <is>
           <t>Equipment Credit</t>
         </is>
       </c>
-      <c r="C6" s="45" t="n">
+      <c r="C6" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="50" t="inlineStr">
+      <c r="D6" s="48" t="inlineStr">
         <is>
           <t>No hardware credits available</t>
         </is>
@@ -1862,200 +1871,200 @@
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>3-Year Summary</t>
         </is>
       </c>
     </row>
     <row r="2" ht="32" customHeight="1">
-      <c r="A2" s="33" t="inlineStr">
+      <c r="A2" s="36" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B2" s="33" t="inlineStr">
+      <c r="B2" s="36" t="inlineStr">
         <is>
           <t>Year 1 List</t>
         </is>
       </c>
-      <c r="C2" s="33" t="inlineStr">
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>Year 1 Credits</t>
         </is>
       </c>
-      <c r="D2" s="33" t="inlineStr">
+      <c r="D2" s="36" t="inlineStr">
         <is>
           <t>Year 1 Net</t>
         </is>
       </c>
-      <c r="E2" s="33" t="inlineStr">
+      <c r="E2" s="36" t="inlineStr">
         <is>
           <t>Year 2</t>
         </is>
       </c>
-      <c r="F2" s="33" t="inlineStr">
+      <c r="F2" s="36" t="inlineStr">
         <is>
           <t>Year 3</t>
         </is>
       </c>
-      <c r="G2" s="33" t="inlineStr">
+      <c r="G2" s="36" t="inlineStr">
         <is>
           <t>3-Year Total</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="20" customHeight="1">
-      <c r="A3" s="38" t="inlineStr">
+    <row r="3" ht="26" customHeight="1">
+      <c r="A3" s="43" t="inlineStr">
         <is>
           <t>Cloud Infrastructure</t>
         </is>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="46">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A3,'Infrastructure Costs'!$G:$G)</f>
         <v/>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="46">
         <f>SUMIF(Credits!$A:$A,A3,Credits!$C:$C)</f>
         <v/>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="46">
         <f>B3+C3</f>
         <v/>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="46">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A3,'Infrastructure Costs'!$H:$H)</f>
         <v/>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="46">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A3,'Infrastructure Costs'!$I:$I)</f>
         <v/>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="46">
         <f>D3+E3+F3</f>
         <v/>
       </c>
     </row>
-    <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="42" t="inlineStr">
+    <row r="4" ht="26" customHeight="1">
+      <c r="A4" s="47" t="inlineStr">
         <is>
           <t>Software Licenses</t>
         </is>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="50">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A4,'Infrastructure Costs'!$G:$G)</f>
         <v/>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="50">
         <f>SUMIF(Credits!$A:$A,A4,Credits!$C:$C)</f>
         <v/>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="50">
         <f>B4+C4</f>
         <v/>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="50">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A4,'Infrastructure Costs'!$H:$H)</f>
         <v/>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="50">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A4,'Infrastructure Costs'!$I:$I)</f>
         <v/>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="50">
         <f>D4+E4+F4</f>
         <v/>
       </c>
     </row>
-    <row r="5" ht="20" customHeight="1">
-      <c r="A5" s="38" t="inlineStr">
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" s="43" t="inlineStr">
         <is>
           <t>Support &amp; Maintenance</t>
         </is>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="46">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A5,'Infrastructure Costs'!$G:$G)</f>
         <v/>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="46">
         <f>SUMIF(Credits!$A:$A,A5,Credits!$C:$C)</f>
         <v/>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="46">
         <f>B5+C5</f>
         <v/>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="46">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A5,'Infrastructure Costs'!$H:$H)</f>
         <v/>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="46">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A5,'Infrastructure Costs'!$I:$I)</f>
         <v/>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="46">
         <f>D5+E5+F5</f>
         <v/>
       </c>
     </row>
-    <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="42" t="inlineStr">
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" s="47" t="inlineStr">
         <is>
           <t>Hardware/Equipment</t>
         </is>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="50">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$G:$G)</f>
         <v/>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="50">
         <f>SUMIF(Credits!$A:$A,A6,Credits!$C:$C)</f>
         <v/>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="50">
         <f>B6+C6</f>
         <v/>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="50">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$H:$H)</f>
         <v/>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="50">
         <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$I:$I)</f>
         <v/>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="50">
         <f>D6+E6+F6</f>
         <v/>
       </c>
     </row>
-    <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="46" t="inlineStr">
+    <row r="7" ht="26" customHeight="1">
+      <c r="A7" s="51" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="53">
         <f>SUM(B3:B6)</f>
         <v/>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="53">
         <f>SUM(C3:C6)</f>
         <v/>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="53">
         <f>SUM(D3:D6)</f>
         <v/>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="53">
         <f>SUM(E3:E6)</f>
         <v/>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="53">
         <f>SUM(F3:F6)</f>
         <v/>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="53">
         <f>SUM(G3:G6)</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Update solution-template to November 2025 infrastructure cost categories
- Standardize categories: Hardware, Cloud Services, Software Licenses,
  Connectivity, Support & Maintenance, Facilities
- Regenerate all presales documents with new category structure
- Add CLAUDE.md to .gitignore
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/presales/infrastructure-costs.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/presales/infrastructure-costs.xlsx
@@ -13,10 +13,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3-Year Summary" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sizing Guidelines'!$A$2:$F$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Infrastructure Costs'!$A$2:$K$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Credits'!$A$2:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3-Year Summary'!$A$2:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sizing Guidelines'!$A$2:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Infrastructure Costs'!$A$2:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Credits'!$A$2:$D$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3-Year Summary'!$A$2:$G$9</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -836,7 +836,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>November 21, 2025</t>
+          <t>November 25, 2025</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -955,128 +955,128 @@
     <row r="3" ht="26" customHeight="1">
       <c r="A3" s="37" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="B3" s="38" t="inlineStr">
         <is>
-          <t>Compute Instances</t>
+          <t>Network Devices</t>
         </is>
       </c>
       <c r="C3" s="39" t="inlineStr">
         <is>
-          <t>2-4 instances</t>
+          <t>0-2 devices</t>
         </is>
       </c>
       <c r="D3" s="39" t="inlineStr">
         <is>
-          <t>5-10 instances</t>
+          <t>3-5 devices</t>
         </is>
       </c>
       <c r="E3" s="39" t="inlineStr">
         <is>
-          <t>15+ instances</t>
+          <t>10+ devices</t>
         </is>
       </c>
       <c r="F3" s="38" t="inlineStr">
         <is>
-          <t>Production workload capacity</t>
+          <t>Based on site count</t>
         </is>
       </c>
     </row>
     <row r="4" ht="26" customHeight="1">
       <c r="A4" s="40" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B4" s="41" t="inlineStr">
         <is>
-          <t>Storage Volume</t>
+          <t>Compute Instances</t>
         </is>
       </c>
       <c r="C4" s="42" t="inlineStr">
         <is>
-          <t>100 GB</t>
+          <t>2-4 instances</t>
         </is>
       </c>
       <c r="D4" s="42" t="inlineStr">
         <is>
-          <t>500 GB - 1 TB</t>
+          <t>5-10 instances</t>
         </is>
       </c>
       <c r="E4" s="42" t="inlineStr">
         <is>
-          <t>2+ TB</t>
+          <t>15+ instances</t>
         </is>
       </c>
       <c r="F4" s="41" t="inlineStr">
         <is>
-          <t>Based on data requirements</t>
+          <t>Production workload capacity</t>
         </is>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
       <c r="A5" s="37" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B5" s="38" t="inlineStr">
         <is>
-          <t>Database Size</t>
+          <t>Storage Volume</t>
         </is>
       </c>
       <c r="C5" s="39" t="inlineStr">
         <is>
-          <t>Small/Standard tier</t>
+          <t>100 GB</t>
         </is>
       </c>
       <c r="D5" s="39" t="inlineStr">
         <is>
-          <t>Medium tier</t>
+          <t>500 GB - 1 TB</t>
         </is>
       </c>
       <c r="E5" s="39" t="inlineStr">
         <is>
-          <t>Large/Enterprise tier</t>
+          <t>2+ TB</t>
         </is>
       </c>
       <c r="F5" s="38" t="inlineStr">
         <is>
-          <t>Based on transaction volume</t>
+          <t>Based on data requirements</t>
         </is>
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
       <c r="A6" s="40" t="inlineStr">
         <is>
-          <t>Software Licenses</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B6" s="41" t="inlineStr">
         <is>
-          <t>User Licenses</t>
+          <t>Database Size</t>
         </is>
       </c>
       <c r="C6" s="42" t="inlineStr">
         <is>
-          <t>10-50 users</t>
+          <t>Small/Standard tier</t>
         </is>
       </c>
       <c r="D6" s="42" t="inlineStr">
         <is>
-          <t>50-250 users</t>
+          <t>Medium tier</t>
         </is>
       </c>
       <c r="E6" s="42" t="inlineStr">
         <is>
-          <t>500+ users</t>
+          <t>Large/Enterprise tier</t>
         </is>
       </c>
       <c r="F6" s="41" t="inlineStr">
         <is>
-          <t>Concurrent or named users</t>
+          <t>Based on transaction volume</t>
         </is>
       </c>
     </row>
@@ -1088,96 +1088,160 @@
       </c>
       <c r="B7" s="38" t="inlineStr">
         <is>
-          <t>Monitoring Tools</t>
+          <t>User Licenses</t>
         </is>
       </c>
       <c r="C7" s="39" t="inlineStr">
         <is>
-          <t>Basic monitoring</t>
+          <t>10-50 users</t>
         </is>
       </c>
       <c r="D7" s="39" t="inlineStr">
         <is>
-          <t>Advanced APM</t>
+          <t>50-250 users</t>
         </is>
       </c>
       <c r="E7" s="39" t="inlineStr">
         <is>
-          <t>Enterprise observability</t>
+          <t>500+ users</t>
         </is>
       </c>
       <c r="F7" s="38" t="inlineStr">
         <is>
-          <t>Application performance monitoring</t>
+          <t>Concurrent or named users</t>
         </is>
       </c>
     </row>
     <row r="8" ht="26" customHeight="1">
       <c r="A8" s="40" t="inlineStr">
         <is>
-          <t>Support &amp; Maintenance</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B8" s="41" t="inlineStr">
         <is>
-          <t>Support Level</t>
+          <t>Monitoring Tools</t>
         </is>
       </c>
       <c r="C8" s="42" t="inlineStr">
         <is>
-          <t>Business hours</t>
+          <t>Basic monitoring</t>
         </is>
       </c>
       <c r="D8" s="42" t="inlineStr">
         <is>
-          <t>24x5 support</t>
+          <t>Advanced APM</t>
         </is>
       </c>
       <c r="E8" s="42" t="inlineStr">
         <is>
-          <t>24x7 premium</t>
+          <t>Enterprise observability</t>
         </is>
       </c>
       <c r="F8" s="41" t="inlineStr">
         <is>
-          <t>SLA requirements</t>
+          <t>Application performance monitoring</t>
         </is>
       </c>
     </row>
     <row r="9" ht="26" customHeight="1">
       <c r="A9" s="37" t="inlineStr">
         <is>
-          <t>Hardware/Equipment</t>
+          <t>Connectivity</t>
         </is>
       </c>
       <c r="B9" s="38" t="inlineStr">
         <is>
-          <t>Network Devices</t>
+          <t>Network Bandwidth</t>
         </is>
       </c>
       <c r="C9" s="39" t="inlineStr">
         <is>
-          <t>0-2 devices</t>
+          <t>100 Mbps</t>
         </is>
       </c>
       <c r="D9" s="39" t="inlineStr">
         <is>
-          <t>3-5 devices</t>
+          <t>500 Mbps</t>
         </is>
       </c>
       <c r="E9" s="39" t="inlineStr">
         <is>
-          <t>10+ devices</t>
+          <t>1+ Gbps</t>
         </is>
       </c>
       <c r="F9" s="38" t="inlineStr">
         <is>
-          <t>Based on site count</t>
+          <t>WAN/Internet circuit speed</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="26" customHeight="1">
+      <c r="A10" s="40" t="inlineStr">
+        <is>
+          <t>Support &amp; Maintenance</t>
+        </is>
+      </c>
+      <c r="B10" s="41" t="inlineStr">
+        <is>
+          <t>Support Level</t>
+        </is>
+      </c>
+      <c r="C10" s="42" t="inlineStr">
+        <is>
+          <t>Business hours</t>
+        </is>
+      </c>
+      <c r="D10" s="42" t="inlineStr">
+        <is>
+          <t>24x5 support</t>
+        </is>
+      </c>
+      <c r="E10" s="42" t="inlineStr">
+        <is>
+          <t>24x7 premium</t>
+        </is>
+      </c>
+      <c r="F10" s="41" t="inlineStr">
+        <is>
+          <t>SLA requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="26" customHeight="1">
+      <c r="A11" s="37" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="B11" s="38" t="inlineStr">
+        <is>
+          <t>Data Center Space</t>
+        </is>
+      </c>
+      <c r="C11" s="39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D11" s="39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" s="39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F11" s="38" t="inlineStr">
+        <is>
+          <t>Cloud-only solution (no facilities)</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F9"/>
+  <autoFilter ref="A2:F11"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
@@ -1191,7 +1255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1280,40 +1344,40 @@
     <row r="3" ht="26" customHeight="1">
       <c r="A3" s="43" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="B3" s="44" t="inlineStr">
         <is>
-          <t>Compute Instance</t>
+          <t>Network Switch</t>
         </is>
       </c>
       <c r="C3" s="44" t="inlineStr">
         <is>
-          <t>Cloud VM or equivalent</t>
+          <t>Network equipment</t>
         </is>
       </c>
       <c r="D3" s="45" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="44" t="inlineStr">
         <is>
-          <t>Instance/Month</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="F3" s="46" t="n">
-        <v>150</v>
+        <v>2500</v>
       </c>
       <c r="G3" s="46">
-        <f>D3*F3*12</f>
+        <f>D3*F3</f>
         <v/>
       </c>
       <c r="H3" s="46">
-        <f>G3</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="I3" s="46">
-        <f>G3</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="J3" s="46">
@@ -1322,28 +1386,28 @@
       </c>
       <c r="K3" s="44" t="inlineStr">
         <is>
-          <t>Production workloads</t>
+          <t>Optional on-premises</t>
         </is>
       </c>
     </row>
     <row r="4" ht="26" customHeight="1">
       <c r="A4" s="47" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B4" s="48" t="inlineStr">
         <is>
-          <t>Database</t>
+          <t>Compute Instance</t>
         </is>
       </c>
       <c r="C4" s="48" t="inlineStr">
         <is>
-          <t>Managed database service</t>
+          <t>Cloud VM or equivalent</t>
         </is>
       </c>
       <c r="D4" s="49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="48" t="inlineStr">
         <is>
@@ -1351,7 +1415,7 @@
         </is>
       </c>
       <c r="F4" s="50" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="G4" s="50">
         <f>D4*F4*12</f>
@@ -1371,36 +1435,36 @@
       </c>
       <c r="K4" s="48" t="inlineStr">
         <is>
-          <t>Relational database</t>
+          <t>Production workloads</t>
         </is>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
       <c r="A5" s="43" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B5" s="44" t="inlineStr">
         <is>
-          <t>Storage</t>
+          <t>Database</t>
         </is>
       </c>
       <c r="C5" s="44" t="inlineStr">
         <is>
-          <t>Object storage</t>
+          <t>Managed database service</t>
         </is>
       </c>
       <c r="D5" s="45" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E5" s="44" t="inlineStr">
         <is>
-          <t>GB/Month</t>
+          <t>Instance/Month</t>
         </is>
       </c>
       <c r="F5" s="46" t="n">
-        <v>0.023</v>
+        <v>200</v>
       </c>
       <c r="G5" s="46">
         <f>D5*F5*12</f>
@@ -1420,28 +1484,28 @@
       </c>
       <c r="K5" s="44" t="inlineStr">
         <is>
-          <t>Data storage</t>
+          <t>Relational database</t>
         </is>
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
       <c r="A6" s="47" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B6" s="48" t="inlineStr">
         <is>
-          <t>Data Transfer</t>
+          <t>Storage</t>
         </is>
       </c>
       <c r="C6" s="48" t="inlineStr">
         <is>
-          <t>Outbound transfer</t>
+          <t>Object storage</t>
         </is>
       </c>
       <c r="D6" s="49" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E6" s="48" t="inlineStr">
         <is>
@@ -1449,7 +1513,7 @@
         </is>
       </c>
       <c r="F6" s="50" t="n">
-        <v>0.09</v>
+        <v>0.023</v>
       </c>
       <c r="G6" s="50">
         <f>D6*F6*12</f>
@@ -1469,36 +1533,36 @@
       </c>
       <c r="K6" s="48" t="inlineStr">
         <is>
-          <t>Egress charges</t>
+          <t>Data storage</t>
         </is>
       </c>
     </row>
     <row r="7" ht="26" customHeight="1">
       <c r="A7" s="43" t="inlineStr">
         <is>
-          <t>Software Licenses</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B7" s="44" t="inlineStr">
         <is>
-          <t>Monitoring</t>
+          <t>Data Transfer</t>
         </is>
       </c>
       <c r="C7" s="44" t="inlineStr">
         <is>
-          <t>Application monitoring</t>
+          <t>Outbound transfer</t>
         </is>
       </c>
       <c r="D7" s="45" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E7" s="44" t="inlineStr">
         <is>
-          <t>Service/Month</t>
+          <t>GB/Month</t>
         </is>
       </c>
       <c r="F7" s="46" t="n">
-        <v>50</v>
+        <v>0.09</v>
       </c>
       <c r="G7" s="46">
         <f>D7*F7*12</f>
@@ -1518,7 +1582,7 @@
       </c>
       <c r="K7" s="44" t="inlineStr">
         <is>
-          <t>Metrics and logging</t>
+          <t>Egress charges</t>
         </is>
       </c>
     </row>
@@ -1530,12 +1594,12 @@
       </c>
       <c r="B8" s="48" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>Monitoring</t>
         </is>
       </c>
       <c r="C8" s="48" t="inlineStr">
         <is>
-          <t>Web application firewall</t>
+          <t>Application monitoring</t>
         </is>
       </c>
       <c r="D8" s="49" t="n">
@@ -1547,7 +1611,7 @@
         </is>
       </c>
       <c r="F8" s="50" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G8" s="50">
         <f>D8*F8*12</f>
@@ -1567,24 +1631,24 @@
       </c>
       <c r="K8" s="48" t="inlineStr">
         <is>
-          <t>Security controls</t>
+          <t>Metrics and logging</t>
         </is>
       </c>
     </row>
     <row r="9" ht="26" customHeight="1">
       <c r="A9" s="43" t="inlineStr">
         <is>
-          <t>Support &amp; Maintenance</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B9" s="44" t="inlineStr">
         <is>
-          <t>Cloud Support</t>
+          <t>Security</t>
         </is>
       </c>
       <c r="C9" s="44" t="inlineStr">
         <is>
-          <t>Provider support plan</t>
+          <t>Web application firewall</t>
         </is>
       </c>
       <c r="D9" s="45" t="n">
@@ -1592,11 +1656,11 @@
       </c>
       <c r="E9" s="44" t="inlineStr">
         <is>
-          <t>Plan/Month</t>
+          <t>Service/Month</t>
         </is>
       </c>
       <c r="F9" s="46" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G9" s="46">
         <f>D9*F9*12</f>
@@ -1616,24 +1680,24 @@
       </c>
       <c r="K9" s="44" t="inlineStr">
         <is>
-          <t>Technical support</t>
+          <t>Security controls</t>
         </is>
       </c>
     </row>
     <row r="10" ht="26" customHeight="1">
       <c r="A10" s="47" t="inlineStr">
         <is>
-          <t>Hardware/Equipment</t>
+          <t>Connectivity</t>
         </is>
       </c>
       <c r="B10" s="48" t="inlineStr">
         <is>
-          <t>Network Switch</t>
+          <t>Internet Circuit</t>
         </is>
       </c>
       <c r="C10" s="48" t="inlineStr">
         <is>
-          <t>Network equipment</t>
+          <t>Business internet</t>
         </is>
       </c>
       <c r="D10" s="49" t="n">
@@ -1641,14 +1705,14 @@
       </c>
       <c r="E10" s="48" t="inlineStr">
         <is>
-          <t>Device</t>
+          <t>Circuit/Month</t>
         </is>
       </c>
       <c r="F10" s="50" t="n">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="G10" s="50">
-        <f>D10*F10</f>
+        <f>D10*F10*12</f>
         <v/>
       </c>
       <c r="H10" s="50">
@@ -1665,41 +1729,139 @@
       </c>
       <c r="K10" s="48" t="inlineStr">
         <is>
-          <t>Optional on-premises</t>
+          <t>Cloud-only (no circuit needed)</t>
         </is>
       </c>
     </row>
     <row r="11" ht="26" customHeight="1">
-      <c r="A11" s="51" t="inlineStr">
+      <c r="A11" s="43" t="inlineStr">
+        <is>
+          <t>Support &amp; Maintenance</t>
+        </is>
+      </c>
+      <c r="B11" s="44" t="inlineStr">
+        <is>
+          <t>Cloud Support</t>
+        </is>
+      </c>
+      <c r="C11" s="44" t="inlineStr">
+        <is>
+          <t>Provider support plan</t>
+        </is>
+      </c>
+      <c r="D11" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="44" t="inlineStr">
+        <is>
+          <t>Plan/Month</t>
+        </is>
+      </c>
+      <c r="F11" s="46" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" s="46">
+        <f>D11*F11*12</f>
+        <v/>
+      </c>
+      <c r="H11" s="46">
+        <f>G11</f>
+        <v/>
+      </c>
+      <c r="I11" s="46">
+        <f>G11</f>
+        <v/>
+      </c>
+      <c r="J11" s="46">
+        <f>G11+H11+I11</f>
+        <v/>
+      </c>
+      <c r="K11" s="44" t="inlineStr">
+        <is>
+          <t>Technical support</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="26" customHeight="1">
+      <c r="A12" s="47" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="B12" s="48" t="inlineStr">
+        <is>
+          <t>Data Center</t>
+        </is>
+      </c>
+      <c r="C12" s="48" t="inlineStr">
+        <is>
+          <t>Rack space and power</t>
+        </is>
+      </c>
+      <c r="D12" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="48" t="inlineStr">
+        <is>
+          <t>Rack/Month</t>
+        </is>
+      </c>
+      <c r="F12" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="50">
+        <f>D12*F12*12</f>
+        <v/>
+      </c>
+      <c r="H12" s="50">
+        <f>G12</f>
+        <v/>
+      </c>
+      <c r="I12" s="50">
+        <f>G12</f>
+        <v/>
+      </c>
+      <c r="J12" s="50">
+        <f>G12+H12+I12</f>
+        <v/>
+      </c>
+      <c r="K12" s="48" t="inlineStr">
+        <is>
+          <t>Cloud-only (no facilities)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="26" customHeight="1">
+      <c r="A13" s="51" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B11" s="52" t="n"/>
-      <c r="C11" s="52" t="n"/>
-      <c r="D11" s="52" t="n"/>
-      <c r="E11" s="52" t="n"/>
-      <c r="F11" s="52" t="n"/>
-      <c r="G11" s="53">
-        <f>SUM(G3:G10)</f>
-        <v/>
-      </c>
-      <c r="H11" s="53">
-        <f>SUM(H3:H10)</f>
-        <v/>
-      </c>
-      <c r="I11" s="53">
-        <f>SUM(I3:I10)</f>
-        <v/>
-      </c>
-      <c r="J11" s="53">
-        <f>SUM(J3:J10)</f>
-        <v/>
-      </c>
-      <c r="K11" s="52" t="n"/>
+      <c r="B13" s="52" t="n"/>
+      <c r="C13" s="52" t="n"/>
+      <c r="D13" s="52" t="n"/>
+      <c r="E13" s="52" t="n"/>
+      <c r="F13" s="52" t="n"/>
+      <c r="G13" s="53">
+        <f>SUM(G3:G12)</f>
+        <v/>
+      </c>
+      <c r="H13" s="53">
+        <f>SUM(H3:H12)</f>
+        <v/>
+      </c>
+      <c r="I13" s="53">
+        <f>SUM(I3:I12)</f>
+        <v/>
+      </c>
+      <c r="J13" s="53">
+        <f>SUM(J3:J12)</f>
+        <v/>
+      </c>
+      <c r="K13" s="52" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K11"/>
+  <autoFilter ref="A2:K13"/>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
@@ -1713,7 +1875,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1760,52 +1922,52 @@
     <row r="3" ht="26" customHeight="1">
       <c r="A3" s="43" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="B3" s="44" t="inlineStr">
         <is>
-          <t>Provider Credit</t>
+          <t>Equipment Credit</t>
         </is>
       </c>
       <c r="C3" s="46" t="n">
-        <v>-1800</v>
+        <v>0</v>
       </c>
       <c r="D3" s="44" t="inlineStr">
         <is>
-          <t>30% credit on eligible compute and database services</t>
+          <t>No hardware credits available</t>
         </is>
       </c>
     </row>
     <row r="4" ht="26" customHeight="1">
       <c r="A4" s="47" t="inlineStr">
         <is>
-          <t>Software Licenses</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B4" s="48" t="inlineStr">
         <is>
-          <t>Partner Credit</t>
+          <t>Provider Credit</t>
         </is>
       </c>
       <c r="C4" s="50" t="n">
-        <v>0</v>
+        <v>-1800</v>
       </c>
       <c r="D4" s="48" t="inlineStr">
         <is>
-          <t>No software credits available</t>
+          <t>30% credit on eligible compute and database services</t>
         </is>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
       <c r="A5" s="43" t="inlineStr">
         <is>
-          <t>Support &amp; Maintenance</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B5" s="44" t="inlineStr">
         <is>
-          <t>Program Credit</t>
+          <t>Partner Credit</t>
         </is>
       </c>
       <c r="C5" s="46" t="n">
@@ -1813,19 +1975,19 @@
       </c>
       <c r="D5" s="44" t="inlineStr">
         <is>
-          <t>No support credits available</t>
+          <t>No software credits available</t>
         </is>
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
       <c r="A6" s="47" t="inlineStr">
         <is>
-          <t>Hardware/Equipment</t>
+          <t>Connectivity</t>
         </is>
       </c>
       <c r="B6" s="48" t="inlineStr">
         <is>
-          <t>Equipment Credit</t>
+          <t>Circuit Credit</t>
         </is>
       </c>
       <c r="C6" s="50" t="n">
@@ -1833,12 +1995,52 @@
       </c>
       <c r="D6" s="48" t="inlineStr">
         <is>
-          <t>No hardware credits available</t>
+          <t>No connectivity credits available</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="26" customHeight="1">
+      <c r="A7" s="43" t="inlineStr">
+        <is>
+          <t>Support &amp; Maintenance</t>
+        </is>
+      </c>
+      <c r="B7" s="44" t="inlineStr">
+        <is>
+          <t>Program Credit</t>
+        </is>
+      </c>
+      <c r="C7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="44" t="inlineStr">
+        <is>
+          <t>No support credits available</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="26" customHeight="1">
+      <c r="A8" s="47" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="B8" s="48" t="inlineStr">
+        <is>
+          <t>Facilities Credit</t>
+        </is>
+      </c>
+      <c r="C8" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="48" t="inlineStr">
+        <is>
+          <t>No facilities (cloud-only solution)</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D6"/>
+  <autoFilter ref="A2:D8"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -1852,7 +2054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1917,7 +2119,7 @@
     <row r="3" ht="26" customHeight="1">
       <c r="A3" s="43" t="inlineStr">
         <is>
-          <t>Cloud Infrastructure</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="B3" s="46">
@@ -1948,7 +2150,7 @@
     <row r="4" ht="26" customHeight="1">
       <c r="A4" s="47" t="inlineStr">
         <is>
-          <t>Software Licenses</t>
+          <t>Cloud Services</t>
         </is>
       </c>
       <c r="B4" s="50">
@@ -1979,7 +2181,7 @@
     <row r="5" ht="26" customHeight="1">
       <c r="A5" s="43" t="inlineStr">
         <is>
-          <t>Support &amp; Maintenance</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B5" s="46">
@@ -2010,7 +2212,7 @@
     <row r="6" ht="26" customHeight="1">
       <c r="A6" s="47" t="inlineStr">
         <is>
-          <t>Hardware/Equipment</t>
+          <t>Connectivity</t>
         </is>
       </c>
       <c r="B6" s="50">
@@ -2039,38 +2241,100 @@
       </c>
     </row>
     <row r="7" ht="26" customHeight="1">
-      <c r="A7" s="51" t="inlineStr">
+      <c r="A7" s="43" t="inlineStr">
+        <is>
+          <t>Support &amp; Maintenance</t>
+        </is>
+      </c>
+      <c r="B7" s="46">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A7,'Infrastructure Costs'!$G:$G)</f>
+        <v/>
+      </c>
+      <c r="C7" s="46">
+        <f>SUMIF(Credits!$A:$A,A7,Credits!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="D7" s="46">
+        <f>B7+C7</f>
+        <v/>
+      </c>
+      <c r="E7" s="46">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A7,'Infrastructure Costs'!$H:$H)</f>
+        <v/>
+      </c>
+      <c r="F7" s="46">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A7,'Infrastructure Costs'!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="G7" s="46">
+        <f>D7+E7+F7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="26" customHeight="1">
+      <c r="A8" s="47" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="B8" s="50">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A8,'Infrastructure Costs'!$G:$G)</f>
+        <v/>
+      </c>
+      <c r="C8" s="50">
+        <f>SUMIF(Credits!$A:$A,A8,Credits!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="D8" s="50">
+        <f>B8+C8</f>
+        <v/>
+      </c>
+      <c r="E8" s="50">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A8,'Infrastructure Costs'!$H:$H)</f>
+        <v/>
+      </c>
+      <c r="F8" s="50">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A8,'Infrastructure Costs'!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="G8" s="50">
+        <f>D8+E8+F8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="26" customHeight="1">
+      <c r="A9" s="51" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B7" s="53">
-        <f>SUM(B3:B6)</f>
-        <v/>
-      </c>
-      <c r="C7" s="53">
-        <f>SUM(C3:C6)</f>
-        <v/>
-      </c>
-      <c r="D7" s="53">
-        <f>SUM(D3:D6)</f>
-        <v/>
-      </c>
-      <c r="E7" s="53">
-        <f>SUM(E3:E6)</f>
-        <v/>
-      </c>
-      <c r="F7" s="53">
-        <f>SUM(F3:F6)</f>
-        <v/>
-      </c>
-      <c r="G7" s="53">
-        <f>SUM(G3:G6)</f>
+      <c r="B9" s="53">
+        <f>SUM(B3:B8)</f>
+        <v/>
+      </c>
+      <c r="C9" s="53">
+        <f>SUM(C3:C8)</f>
+        <v/>
+      </c>
+      <c r="D9" s="53">
+        <f>SUM(D3:D8)</f>
+        <v/>
+      </c>
+      <c r="E9" s="53">
+        <f>SUM(E3:E8)</f>
+        <v/>
+      </c>
+      <c r="F9" s="53">
+        <f>SUM(F3:F8)</f>
+        <v/>
+      </c>
+      <c r="G9" s="53">
+        <f>SUM(G3:G8)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G7"/>
+  <autoFilter ref="A2:G9"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>